<commit_message>
Adding architectural constraints and ICSA use cases
</commit_message>
<xml_diff>
--- a/timetracking/TimeTracking.xlsx
+++ b/timetracking/TimeTracking.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmilo/Documents/PhD/Sem6/journal ss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kmilo/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dev&amp;DepTimes" sheetId="3" r:id="rId1"/>
     <sheet name="Dev&amp;Dep4Iter" sheetId="4" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -293,7 +296,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dev&amp;Dep4Iter'!$A$2:$A$4</c:f>
+              <c:f>'Dev&amp;Dep4Iter'!$A$3:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -370,7 +373,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dev&amp;Dep4Iter'!$A$2:$A$4</c:f>
+              <c:f>'Dev&amp;Dep4Iter'!$A$3:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -446,7 +449,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dev&amp;Dep4Iter'!$A$2:$A$4</c:f>
+              <c:f>'Dev&amp;Dep4Iter'!$A$3:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -490,11 +493,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1737396032"/>
-        <c:axId val="-1702486640"/>
+        <c:axId val="288302016"/>
+        <c:axId val="290925056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1737396032"/>
+        <c:axId val="288302016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.0"/>
@@ -595,13 +598,13 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1702486640"/>
+        <c:crossAx val="290925056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1702486640"/>
+        <c:axId val="290925056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -707,7 +710,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1737396032"/>
+        <c:crossAx val="288302016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -910,7 +913,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dev&amp;Dep4Iter'!$A$16:$A$18</c:f>
+              <c:f>'Dev&amp;Dep4Iter'!$A$12:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -987,7 +990,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dev&amp;Dep4Iter'!$A$16:$A$18</c:f>
+              <c:f>'Dev&amp;Dep4Iter'!$A$12:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1063,7 +1066,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Dev&amp;Dep4Iter'!$A$16:$A$18</c:f>
+              <c:f>'Dev&amp;Dep4Iter'!$A$12:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1107,11 +1110,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1702524976"/>
-        <c:axId val="-1702521856"/>
+        <c:axId val="685307008"/>
+        <c:axId val="254760560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1702524976"/>
+        <c:axId val="685307008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.0"/>
@@ -1206,13 +1209,13 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1702521856"/>
+        <c:crossAx val="254760560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1702521856"/>
+        <c:axId val="254760560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -1289,6 +1292,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1319,7 +1323,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1702524976"/>
+        <c:crossAx val="685307008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2577,6 +2581,103 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Hoja1"/>
+      <sheetName val="Hoja2"/>
+      <sheetName val="JSS"/>
+      <sheetName val="Hoja4"/>
+      <sheetName val="ICSA20"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="31">
+          <cell r="T31" t="str">
+            <v>SpringXD</v>
+          </cell>
+          <cell r="U31" t="str">
+            <v>FastScore</v>
+          </cell>
+          <cell r="V31" t="str">
+            <v>ACCORDANT</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="S33" t="str">
+            <v>UC1</v>
+          </cell>
+          <cell r="T33">
+            <v>11.25</v>
+          </cell>
+          <cell r="U33">
+            <v>11.5</v>
+          </cell>
+          <cell r="V33">
+            <v>16.25</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="S34" t="str">
+            <v>UC2</v>
+          </cell>
+          <cell r="T34">
+            <v>5</v>
+          </cell>
+          <cell r="U34">
+            <v>5.5</v>
+          </cell>
+          <cell r="V34">
+            <v>6.75</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="T38" t="str">
+            <v>SpringXD</v>
+          </cell>
+          <cell r="U38" t="str">
+            <v>FastScore</v>
+          </cell>
+          <cell r="V38" t="str">
+            <v>ACCORDANT</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="T40">
+            <v>8.25</v>
+          </cell>
+          <cell r="U40">
+            <v>7.5</v>
+          </cell>
+          <cell r="V40">
+            <v>1.5</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="S41" t="str">
+            <v>UC2</v>
+          </cell>
+          <cell r="T41">
+            <v>4</v>
+          </cell>
+          <cell r="U41">
+            <v>4</v>
+          </cell>
+          <cell r="V41">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -2842,8 +2943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2934,22 +3035,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2.75</v>
+        <v>5.25</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>8.25</v>
       </c>
       <c r="E4">
-        <v>2.25</v>
+        <v>4.25</v>
       </c>
       <c r="F4">
-        <v>2.5</v>
+        <v>4.25</v>
       </c>
       <c r="G4">
-        <v>2.75</v>
+        <v>5.75</v>
       </c>
       <c r="H4">
         <v>1.75</v>
@@ -2966,22 +3067,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.25</v>
+        <v>2.75</v>
       </c>
       <c r="C5">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>8.25</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>4.25</v>
+        <v>2.25</v>
       </c>
       <c r="F5">
-        <v>4.25</v>
+        <v>2.5</v>
       </c>
       <c r="G5">
-        <v>5.75</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -3161,10 +3262,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3178,9 +3279,6 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -3193,7 +3291,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2.875</v>
@@ -3207,7 +3305,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2.3125</v>
@@ -3220,6 +3318,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5">
         <v>1.375</v>
       </c>
@@ -3236,6 +3337,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -3247,6 +3351,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
       <c r="B12">
         <v>2.75</v>
       </c>
@@ -3258,6 +3365,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
       <c r="B13">
         <v>1.8125</v>
       </c>
@@ -3269,6 +3379,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3</v>
+      </c>
       <c r="B14">
         <v>1.875</v>
       </c>
@@ -3277,26 +3390,6 @@
       </c>
       <c r="D14">
         <v>0.375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>